<commit_message>
update tianyan inst 1
</commit_message>
<xml_diff>
--- a/data-raw/data-tidy/hack-tianyan/hub/match-tianyan-tot4-2022-08-19-hand.xlsx
+++ b/data-raw/data-tidy/hack-tianyan/hub/match-tianyan-tot4-2022-08-19-hand.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\techme\data-raw\data-tidy\hack-tianyan\hub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F7DA8F-B8A1-49A2-9190-D9550AE3FD2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4661A0F-69E1-414B-B8CD-58F1678A59DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9892" yWindow="8258" windowWidth="24495" windowHeight="15674" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="20">
   <si>
     <t>index</t>
   </si>
@@ -75,6 +75,17 @@
   </si>
   <si>
     <t>010-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中国农科院农产品加工研究所</t>
+  </si>
+  <si>
+    <t>中国农科院农产品加工研究所</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北京市海淀区</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -82,7 +93,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -112,6 +123,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -133,11 +151,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -434,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,6 +598,29 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>